<commit_message>
correct error in measure degree distribution
</commit_message>
<xml_diff>
--- a/task2/degree_distribution.xlsx
+++ b/task2/degree_distribution.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,7 +450,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -474,119 +474,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>16</v>
-      </c>
-      <c r="B17" t="n">
         <v>2</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>